<commit_message>
reload obs nota credito
</commit_message>
<xml_diff>
--- a/recursos/FALTANTES CONSORCIO_21122022.xlsx
+++ b/recursos/FALTANTES CONSORCIO_21122022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevFiles\xampps\7.0.32\htdocs\consorcio_test\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CD9833-3EBC-4296-AB9A-B49CC874957A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A80DD4B-4252-48E2-B392-57B44847B5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -391,6 +391,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -709,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +745,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="12" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="10">
@@ -1223,7 +1226,7 @@
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="11" t="s">
         <v>68</v>
       </c>
       <c r="D45" s="8">
@@ -1234,7 +1237,7 @@
       </c>
     </row>
     <row r="46" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="11" t="s">
         <v>69</v>
       </c>
       <c r="D46" s="8">

</xml_diff>